<commit_message>
EBEGU-415 * cleaning up and adding test data * adding excel formatting
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -14,9 +14,6 @@
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="GesuchStichtagPivottableData">Data!$A$1:$G$2</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -90,6 +87,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -119,8 +120,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,7 +442,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,22 +498,22 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="J2" t="s">
@@ -518,6 +522,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
EBEGU-949 - Der Excel wurde eine neue Spalte "Ignoriert" hinzugefuegt. Dies gilt sowohl fuer die neue Zahlungen bzw. zeitabschnitte als auch fuer die alten. Aus diesem Grund reicht nicht aus, den Status der alte Abschnitt zu holen, da er VERRECHNET ist und nicht ignoriert. Man muss den alten Zeitabschnitt als Ignoriert markieren, wenn der neue Abschnitt ignoriert ist  - Nun werden fuer die Zahlungen nicht nur alle neuen (isNeu()) Zeitabschnitte berechnet, sondern alle die nicht verrechnet sind. Dies wird gebraucht, um ignorierte Zeitabschnitte in der Excel zu zeigen  - Methode isAuszuzahlen() wurde entfernt, da sie keinen Sinn mehr macht. Dies war Teil einer alten Loesung, die wir nicht implementieren werden. Anstatt dessen muss man schauen ob die Zahlungsposition ignoriert ist
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\medu\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="2925" yWindow="1080" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Institution</t>
   </si>
@@ -81,15 +81,22 @@
   </si>
   <si>
     <t>Betrag in CHF</t>
+  </si>
+  <si>
+    <t>In Zahlungslauf
+ignorieren</t>
+  </si>
+  <si>
+    <t>{isIgnoriert}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -120,14 +127,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -439,56 +455,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="J1" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -516,7 +536,10 @@
       <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
EBEGU-949 - Status IGNORIERT wurde in IGNORIEREND und IGNORIERT getrennt. Der Status IGNORIEREND heisst, dass der Zeitabschnitt bei der nächsten Zahlung als IGNORIERT behandelt werden muss. Wenn diese Zeitabschnitt ausbezahlt wurde, aendert der Status auf IGNORIERT. Ein Zeitabschnitt im Status IGNORIERT wird in zukuenftigen Zahlungen nicht beruecksichtigt -> So unterscheiden wir zwischen Zeitabschnitte die man ignorieren muss und Zeitabschnitt die bereits ignoriert wurden. - Die Excel ZahlungAuftrag wurde angepasst: -- Die Zeilen werden nun auch bei BGID sortiert -- Eine neue boolean Spalte isKorrektur wurde hinzugefuegt. -- Die Zeilen die Korrekturen sind, haben fontcolor = rot.
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2925" yWindow="1080" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="7800" yWindow="2880" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Institution</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>{isIgnoriert}</t>
+  </si>
+  <si>
+    <t>Korrektur</t>
+  </si>
+  <si>
+    <t>{isKorrektur}</t>
   </si>
 </sst>
 </file>
@@ -127,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -141,11 +147,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -455,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
@@ -471,12 +486,12 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -504,11 +519,14 @@
       <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -536,14 +554,22 @@
       <c r="I2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:XFD99999">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$J$2="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
EBEGU-949 - Excel Zahlungsauftrag verbessert. Jetzt hat es etwas styling und die Daten generiert und faellig werden angezeigt
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2880" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="11700" yWindow="4320" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Institution</t>
   </si>
@@ -94,6 +94,21 @@
   </si>
   <si>
     <t>{isKorrektur}</t>
+  </si>
+  <si>
+    <t>{beschrieb}</t>
+  </si>
+  <si>
+    <t>{generiertAm}</t>
+  </si>
+  <si>
+    <t>{faelligAm}</t>
+  </si>
+  <si>
+    <t>generiert am</t>
+  </si>
+  <si>
+    <t>faellig am</t>
   </si>
 </sst>
 </file>
@@ -104,7 +119,7 @@
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$CHF]\ #,##0.00;[Red]\-[$CHF]\ #,##0.00"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,16 +127,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -129,32 +164,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -470,104 +534,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L7" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:XFD99999">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$J$2="X"</formula>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A7:XFD18 A21:XFD100004 C19:XFD20">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$J7="X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A3:B4">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$J19="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
EBEGU-949 - neues Feld sameVerguenstigung fuer die Zeitabschnitte. Dieses Feld wird gebraucht, um zu wissen, ob der neue Zeitabschnitte eine andere Verguenstigung hat als der alte Zeitabschnitt. Es reicht nicht mit sameVerfuegungsdaten, da fuer die Zahlungen nur die Verguenstigung relevant ist. Es koennte sein dass alle Werte sich geaendert haben aber die verguenstigung nicht, in diesem Fall muss nach Korrektur fuer die Zahlung nicht gefragt werden
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/ZahlungAuftrag.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="4320" windowWidth="28800" windowHeight="14010"/>
+    <workbookView xWindow="12675" yWindow="4680" windowWidth="28800" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -213,7 +213,22 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -537,7 +552,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,14 +682,9 @@
   <mergeCells count="1">
     <mergeCell ref="A1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="A7:XFD18 A21:XFD100004 C19:XFD20">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A7:XFD999999">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$J7="X"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3:B4">
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>$J19="X"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>